<commit_message>
made freebie editable through admin dashboard
</commit_message>
<xml_diff>
--- a/menu-items.xlsx
+++ b/menu-items.xlsx
@@ -409,6 +409,9 @@
       <c r="B1" t="str">
         <v>Flavours Fusion 2025</v>
       </c>
+      <c r="C1">
+        <v>0.03</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -447,7 +450,7 @@
         <v>30</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
background audio and reveal animation added
</commit_message>
<xml_diff>
--- a/menu-items.xlsx
+++ b/menu-items.xlsx
@@ -410,7 +410,7 @@
         <v>Flavours Fusion 2025</v>
       </c>
       <c r="C1">
-        <v>0.03</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -450,7 +450,7 @@
         <v>30</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">

</xml_diff>